<commit_message>
continuing improvements to the code.
</commit_message>
<xml_diff>
--- a/data-raw/queries.xlsx
+++ b/data-raw/queries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA88D2BC-49CC-A04E-9AD0-5D98F0E6B9E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F8728-21CD-A247-B40F-C0A93FC512F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27640" yWindow="4060" windowWidth="27640" windowHeight="16940" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
+    <workbookView xWindow="3920" yWindow="1400" windowWidth="27640" windowHeight="16940" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="128">
   <si>
     <t>food</t>
   </si>
@@ -67,9 +67,6 @@
     <t>FACEozone</t>
   </si>
   <si>
-    <t>IIASAPIKetcPubs</t>
-  </si>
-  <si>
     <t>priceVar</t>
   </si>
   <si>
@@ -665,12 +662,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">(AUTHLASTNAME( Valin  or Havlik  or Pope  or van Meijl  or Sands )  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">land AND ocean AND (conflict OR adaptation OR use OR mitigation) </t>
-  </si>
-  <si>
     <t>livestock*</t>
   </si>
   <si>
@@ -710,9 +701,6 @@
     <t>"free air carbon dioxide" experiment*</t>
   </si>
   <si>
-    <t>agriculture AND ( SSP OR "shared socioeconomic profile*" OR RCP OR "representative concentration pathway*")</t>
-  </si>
-  <si>
     <t>"storage loss" AND (crop OR livestock or fish)</t>
   </si>
   <si>
@@ -738,13 +726,106 @@
   </si>
   <si>
     <t>nutrition* OR nutrition* status OR nutrition* outcome* OR nutrition* health OR anthropometry OR diet</t>
+  </si>
+  <si>
+    <t>medicinalPlants</t>
+  </si>
+  <si>
+    <t>fibre</t>
+  </si>
+  <si>
+    <t>biofuels</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>Fisheries OR fishing OR fish resource OR fish products OR Aquaculture OR Aquacultural</t>
+  </si>
+  <si>
+    <t>croppingSystem</t>
+  </si>
+  <si>
+    <t>cropping  AND system  OR  crops </t>
+  </si>
+  <si>
+    <t>wheat</t>
+  </si>
+  <si>
+    <t>sugarcane</t>
+  </si>
+  <si>
+    <t>sugarc*</t>
+  </si>
+  <si>
+    <t>maize</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>soybean</t>
+  </si>
+  <si>
+    <t>ozonecrop</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>QueryID</t>
+  </si>
+  <si>
+    <t>fertsustain</t>
+  </si>
+  <si>
+    <t>fertilizer AND (crop OR agriculture) AND sustainability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">land AND ocean AND (conflict OR adaptation OR use ) </t>
+  </si>
+  <si>
+    <t>disaster OR flood OR drought OR hurricane OR storm OR cyclone OR "sea level rise" OR "irregular rainfall" OR "intense rainfall"</t>
+  </si>
+  <si>
+    <t>adaptation OR maladaptation OR adaptive OR "adaptive capacity" OR "disaster risk management" OR "risk sharing" OR "risk spreading"</t>
+  </si>
+  <si>
+    <t>consumption OR consum* OR "dietary choice" OR "diet" OR "food choice" OR "food utilisation" OR "food utilization"</t>
+  </si>
+  <si>
+    <t>vulnerability</t>
+  </si>
+  <si>
+    <t>adaptation</t>
+  </si>
+  <si>
+    <t>adaptation2</t>
+  </si>
+  <si>
+    <t>consumption</t>
+  </si>
+  <si>
+    <t>food or fiber</t>
+  </si>
+  <si>
+    <t>agriculture AND ( SSP OR "shared socioeconomic profile*" OR RCP OR "representative concentration pathway")</t>
+  </si>
+  <si>
+    <t>crop AND (ozone or "air quality")</t>
+  </si>
+  <si>
+    <t>"medicinal plants"</t>
+  </si>
+  <si>
+    <t>(insurance OR "social protection" OR education OR learning OR cooperation OR collaboration OR migration OR displacement OR "climate services" OR "climate information") OR ("food system" AND (sustain* OR transition* OR transform*))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -794,6 +875,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -816,14 +904,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1139,181 +1229,437 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F86CE5-FC64-FA44-BB0B-0B6C961403B7}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="10.83203125" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>109</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="C34" s="6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>120</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>119</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C56" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1329,338 +1675,338 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="26" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+    <row r="16" spans="1:1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A95" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="4" t="s">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" s="4" t="s">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="4" t="s">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
+    <row r="115" spans="1:1" ht="23" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A115" s="6" t="s">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="5" t="s">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding a readme file
</commit_message>
<xml_diff>
--- a/data-raw/queries.xlsx
+++ b/data-raw/queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F8728-21CD-A247-B40F-C0A93FC512F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E83D84-BCB1-FB40-B149-1D3319521185}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3920" yWindow="1400" windowWidth="27640" windowHeight="16940" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
   </bookViews>
@@ -773,9 +773,6 @@
     <t>rice</t>
   </si>
   <si>
-    <t>QueryID</t>
-  </si>
-  <si>
     <t>fertsustain</t>
   </si>
   <si>
@@ -819,6 +816,9 @@
   </si>
   <si>
     <t>(insurance OR "social protection" OR education OR learning OR cooperation OR collaboration OR migration OR displacement OR "climate services" OR "climate information") OR ("food system" AND (sustain* OR transition* OR transform*))</t>
+  </si>
+  <si>
+    <t>queryNumber</t>
   </si>
 </sst>
 </file>
@@ -1231,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F86CE5-FC64-FA44-BB0B-0B6C961403B7}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1242,7 +1242,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1424,7 +1424,7 @@
         <v>86</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1468,7 +1468,7 @@
         <v>97</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1479,7 +1479,7 @@
         <v>98</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1589,7 +1589,7 @@
         <v>110</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1597,10 +1597,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1611,7 +1611,7 @@
         <v>7</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1619,10 +1619,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1630,10 +1630,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1641,10 +1641,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1652,10 +1652,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Continued improvements to the code. The queries.xlsx file is now where the number and nature of search columns are determined
</commit_message>
<xml_diff>
--- a/data-raw/queries.xlsx
+++ b/data-raw/queries.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E83D84-BCB1-FB40-B149-1D3319521185}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEBAEA8-D257-4D4D-BF0F-4D742EEE91A6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3920" yWindow="1400" windowWidth="27640" windowHeight="16940" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
+    <workbookView xWindow="79960" yWindow="11260" windowWidth="27640" windowHeight="19500" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="WOS Search Operators_x000a__x000a_Sear" sheetId="2" r:id="rId2"/>
+    <sheet name="Queries" sheetId="1" r:id="rId1"/>
+    <sheet name="searchTerms" sheetId="3" r:id="rId2"/>
+    <sheet name="WOSSearchOperators" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Queries!$A$1:$E$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -32,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="128">
-  <si>
-    <t>food</t>
-  </si>
-  <si>
-    <t>livestock</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="192">
   <si>
     <t>valueChain</t>
   </si>
@@ -52,12 +50,6 @@
     <t>storageLoss</t>
   </si>
   <si>
-    <t>geneticEng</t>
-  </si>
-  <si>
-    <t>impacts</t>
-  </si>
-  <si>
     <t>fruitImpact</t>
   </si>
   <si>
@@ -662,21 +654,12 @@
     </r>
   </si>
   <si>
-    <t>livestock*</t>
-  </si>
-  <si>
     <t>"food value chain"</t>
   </si>
   <si>
     <t xml:space="preserve"> financialization AND agriculture</t>
   </si>
   <si>
-    <t xml:space="preserve">genet* AND (crop OR livestock OR fish)  </t>
-  </si>
-  <si>
-    <t>impact* AND (crop OR livestock OR fish)</t>
-  </si>
-  <si>
     <t>impact* AND (frui* OR tomato* OR strawberr* OR blueberr* OR raspberr* OR grap*)</t>
   </si>
   <si>
@@ -716,18 +699,9 @@
     <t>foodSecurity</t>
   </si>
   <si>
-    <t>food AND (suppl* OR *securit* OR access* OR afford* OR insecur* OR *sufficien* OR desert* OR choice* OR availab* OR intake OR utiliz* OR stabil* OR quality OR poverty)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> "international trade" AND (agriculture OR food)</t>
-  </si>
-  <si>
     <t>nutrition</t>
   </si>
   <si>
-    <t>nutrition* OR nutrition* status OR nutrition* outcome* OR nutrition* health OR anthropometry OR diet</t>
-  </si>
-  <si>
     <t>medicinalPlants</t>
   </si>
   <si>
@@ -740,15 +714,9 @@
     <t>fish</t>
   </si>
   <si>
-    <t>Fisheries OR fishing OR fish resource OR fish products OR Aquaculture OR Aquacultural</t>
-  </si>
-  <si>
     <t>croppingSystem</t>
   </si>
   <si>
-    <t>cropping  AND system  OR  crops </t>
-  </si>
-  <si>
     <t>wheat</t>
   </si>
   <si>
@@ -773,24 +741,6 @@
     <t>rice</t>
   </si>
   <si>
-    <t>fertsustain</t>
-  </si>
-  <si>
-    <t>fertilizer AND (crop OR agriculture) AND sustainability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">land AND ocean AND (conflict OR adaptation OR use ) </t>
-  </si>
-  <si>
-    <t>disaster OR flood OR drought OR hurricane OR storm OR cyclone OR "sea level rise" OR "irregular rainfall" OR "intense rainfall"</t>
-  </si>
-  <si>
-    <t>adaptation OR maladaptation OR adaptive OR "adaptive capacity" OR "disaster risk management" OR "risk sharing" OR "risk spreading"</t>
-  </si>
-  <si>
-    <t>consumption OR consum* OR "dietary choice" OR "diet" OR "food choice" OR "food utilisation" OR "food utilization"</t>
-  </si>
-  <si>
     <t>vulnerability</t>
   </si>
   <si>
@@ -803,29 +753,275 @@
     <t>consumption</t>
   </si>
   <si>
-    <t>food or fiber</t>
-  </si>
-  <si>
     <t>agriculture AND ( SSP OR "shared socioeconomic profile*" OR RCP OR "representative concentration pathway")</t>
   </si>
   <si>
     <t>crop AND (ozone or "air quality")</t>
   </si>
   <si>
-    <t>"medicinal plants"</t>
-  </si>
-  <si>
-    <t>(insurance OR "social protection" OR education OR learning OR cooperation OR collaboration OR migration OR displacement OR "climate services" OR "climate information") OR ("food system" AND (sustain* OR transition* OR transform*))</t>
-  </si>
-  <si>
     <t>queryNumber</t>
+  </si>
+  <si>
+    <t>aquaculture</t>
+  </si>
+  <si>
+    <t>Aquaculture OR Aquacultural</t>
+  </si>
+  <si>
+    <t>"medicinal plant*" OR "wild edible*" OR "aquatic algae" or "aromatic plant*" OR seaweed*</t>
+  </si>
+  <si>
+    <t>sectionName</t>
+  </si>
+  <si>
+    <t>sectionDescription</t>
+  </si>
+  <si>
+    <t>5.3.2 Aquatic systems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.3.3 Aquaculture systems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.3.1 Terrestrial Systems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.5 Climate Change and the Food System Value Chain: from Postharvest to Food </t>
+  </si>
+  <si>
+    <t>geneticEngCrop</t>
+  </si>
+  <si>
+    <t>('genet* AND crop*)</t>
+  </si>
+  <si>
+    <t>geneticEngFish</t>
+  </si>
+  <si>
+    <t>geneticEngLivestock</t>
+  </si>
+  <si>
+    <t>('genet* AND livestoc*)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.2.1 Methodologies for assessing impacts and risks </t>
+  </si>
+  <si>
+    <t>biofuel* OR bioenergy OR agrofuel* OR BECCS OR "bioenergy with carbon capture and storage"</t>
+  </si>
+  <si>
+    <t>"international trade" AND (agriculture OR food)</t>
+  </si>
+  <si>
+    <t>food AND (nutrition* OR nutrition* status OR nutrition* outcome* OR nutrition* health OR anthropometry OR diet)</t>
+  </si>
+  <si>
+    <t>impactsCrop</t>
+  </si>
+  <si>
+    <t>impactsLivestock</t>
+  </si>
+  <si>
+    <t>impact* AND livestock</t>
+  </si>
+  <si>
+    <t>impact* AND fish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.7.1 Food security and climate change </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.7.2 Current state of food security and nutrition (FSN) including over &amp; undernutrition </t>
+  </si>
+  <si>
+    <t>impactsGeneral</t>
+  </si>
+  <si>
+    <t>pests</t>
+  </si>
+  <si>
+    <t>crop AND (pest* OR insect* or fung* OR weed* )</t>
+  </si>
+  <si>
+    <t>grainQuality</t>
+  </si>
+  <si>
+    <t>"grain quality"</t>
+  </si>
+  <si>
+    <t>livestockSystems</t>
+  </si>
+  <si>
+    <t>pastureForage</t>
+  </si>
+  <si>
+    <t>livestockDisease</t>
+  </si>
+  <si>
+    <t>livestock AND disease</t>
+  </si>
+  <si>
+    <t>forestrySystems</t>
+  </si>
+  <si>
+    <t>"*forestry system*"</t>
+  </si>
+  <si>
+    <t>genet* AND fish*</t>
+  </si>
+  <si>
+    <t>impactsFish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.8.2 Global / regional adaptation effectiveness </t>
+  </si>
+  <si>
+    <t>5.7.6 Transitioning to sustainable food systems in the face of climate change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.8.6 Policy implementation </t>
+  </si>
+  <si>
+    <t>searchStrings.RCP</t>
+  </si>
+  <si>
+    <t>searchStrings.SSP</t>
+  </si>
+  <si>
+    <t>searchStrings.regions</t>
+  </si>
+  <si>
+    <t>searchStrings.climateChange</t>
+  </si>
+  <si>
+    <t>c("impact*", "adapt*", "mitigat*")</t>
+  </si>
+  <si>
+    <t>searchStrings.animals</t>
+  </si>
+  <si>
+    <t>searchStrings.cereals</t>
+  </si>
+  <si>
+    <t>c("cereal*", "rice", "maize", "corn", "wheat", "sorghum", "millet")</t>
+  </si>
+  <si>
+    <t>searchStrings.fruits</t>
+  </si>
+  <si>
+    <t>c("frui*", "tomato*", "strawberr*", "blueberr*", "raspberr*", "grap*")</t>
+  </si>
+  <si>
+    <t>searchStrings.vegetables</t>
+  </si>
+  <si>
+    <t>searchStrings.roots</t>
+  </si>
+  <si>
+    <t>searchStrings.stimulants</t>
+  </si>
+  <si>
+    <t>c("coffee", "cocoa", "tea")</t>
+  </si>
+  <si>
+    <t>searchStrings.fish</t>
+  </si>
+  <si>
+    <t>c("fish", "seafood", "molluscs", "salmon", "tuna", "hake")</t>
+  </si>
+  <si>
+    <t>searchStrings.foodSec</t>
+  </si>
+  <si>
+    <t>searchStrings.notPeerRev</t>
+  </si>
+  <si>
+    <t>searchStrings.timePeriod</t>
+  </si>
+  <si>
+    <t>c("*century", "mid century", "end century", "2030", "2025", "2050", "2080", "2100")</t>
+  </si>
+  <si>
+    <t>searchStrings.econ</t>
+  </si>
+  <si>
+    <t>c("food security", "food insecure*",  "food access*", "food sufficien*", "food insufficien*","food stability")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c("RCP", "RCP2.6", "RCP6.0", "RCP4.5", "RCP8.5", "CMIP", "SRES") </t>
+  </si>
+  <si>
+    <t>c("SSP",  "SSP1", "SSP2", "SSP3", "SSP4","SSP5")</t>
+  </si>
+  <si>
+    <t>c("Conference Proceeding", "Letter",  "Correction", "Editorial Material")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c("Latin America", "Central America", "Caribbean",  "Europe", "Northern Europe", "Western Europe", "Southern Europe", "Eastern Europe", "Western Asia", "Middle East","Asia", "South Asia", "East Asia", "Central Asia", "Australia", "New Zealand","Southeast Asia", "Africa", "East Africa", "West Africa", "Central Africa", "North Africa") </t>
+  </si>
+  <si>
+    <t>c("veget*", "caulif*", "tomato*", "bean*", "pea")</t>
+  </si>
+  <si>
+    <t>c("cassava", "yam", "potato", "sweet potato")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c("profit*", "financ*", "economic*", "price", "price variability") </t>
+  </si>
+  <si>
+    <t>c("ruminant", " , "cattle", "beef", "goat", "sheep", "pig", "swine",   "pork", "chicken", "poultry")</t>
+  </si>
+  <si>
+    <t>searchStringName</t>
+  </si>
+  <si>
+    <t>searchString</t>
+  </si>
+  <si>
+    <t>"livestock systems" OR "pastoral systems"</t>
+  </si>
+  <si>
+    <t>maladaptation</t>
+  </si>
+  <si>
+    <t>consum* OR "dietary choice" OR "food choice"</t>
+  </si>
+  <si>
+    <t>fiber OR fibre</t>
+  </si>
+  <si>
+    <t>livestock AND (rangeland OR feed OR forag*)</t>
+  </si>
+  <si>
+    <t>( flood OR drought OR storm OR "sea level rise" OR "extreme event" OR "heat wave") AND crop*</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> flood OR drought OR "sea level rise" OR "extreme event" OR "heat wave"</t>
+  </si>
+  <si>
+    <t>food AND (*securit* OR access* OR afford* OR insecur* OR *sufficien* OR choice* OR availab* OR utiliz* OR stabil* OR quality)</t>
+  </si>
+  <si>
+    <t>adaptation OR adaptive OR "adaptive capacity" OR "risk sharing" OR "risk spreading"</t>
+  </si>
+  <si>
+    <t>Fisheries OR fishing OR "fish resource" OR "fish products"</t>
+  </si>
+  <si>
+    <t>food AND vulnerability</t>
+  </si>
+  <si>
+    <t>"social protection" OR cooperation OR migration OR "climate services" OR "climate information"</t>
+  </si>
+  <si>
+    <t>"cropping system" AND cereal*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -882,6 +1078,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -904,16 +1107,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1229,784 +1448,1183 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F86CE5-FC64-FA44-BB0B-0B6C961403B7}">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" style="6"/>
+    <col min="2" max="2" width="30.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
+        <v>106</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E11" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B16" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="9" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>92</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>102</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="10" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
-        <v>119</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>121</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
-        <v>118</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C56" s="7"/>
+      <c r="B38" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>42</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>43</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>44</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>45</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E65" s="11"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E1" xr:uid="{EB323E7F-C5BD-C24A-9909-3B5183F7D633}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E47">
+      <sortCondition ref="B1:B47"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B44446-4EFF-1748-B076-59F83F2A5201}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>157</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>158</v>
+      </c>
+      <c r="B10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B15" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" t="s">
+        <v>175</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652E5710-150B-C14C-9032-4451AF876B8C}">
   <dimension ref="A1:A121"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="23" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="23" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="23" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="23" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small tweaks leads to code that runs through 45 query results
</commit_message>
<xml_diff>
--- a/data-raw/queries.xlsx
+++ b/data-raw/queries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C09534-F426-834A-9678-B4FFABE4AA06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11DC0A1-0BF5-4E45-96EF-A8556CDA3797}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41580" yWindow="680" windowWidth="27640" windowHeight="19500" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
+    <workbookView xWindow="41580" yWindow="680" windowWidth="27640" windowHeight="19500" activeTab="1" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Queries" sheetId="1" r:id="rId1"/>
@@ -941,9 +941,6 @@
     <t xml:space="preserve">c("profit*", "financ*", "economic*", "price", "price variability") </t>
   </si>
   <si>
-    <t>c("ruminant", " , "cattle", "beef", "goat", "sheep", "pig", "swine",   "pork", "chicken", "poultry")</t>
-  </si>
-  <si>
     <t>searchStringName</t>
   </si>
   <si>
@@ -5222,6 +5219,9 @@
   </si>
   <si>
     <t>legume* OR bean* OR pulses OR pea OR lentil OR chickpea OR cowpea OR "pigeon pea" OR "pigeonpea"</t>
+  </si>
+  <si>
+    <t>c("ruminant",  "cattle", "beef", "goat", "sheep", "pig", "swine",   "pork", "chicken", "poultry")</t>
   </si>
 </sst>
 </file>
@@ -5378,9 +5378,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5698,8 +5698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F86CE5-FC64-FA44-BB0B-0B6C961403B7}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5738,7 +5738,7 @@
         <v>77</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -5753,7 +5753,7 @@
         <v>131</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -5783,7 +5783,7 @@
         <v>132</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -5825,10 +5825,10 @@
         <v>110</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -5888,7 +5888,7 @@
         <v>86</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -5918,7 +5918,7 @@
         <v>89</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5975,10 +5975,10 @@
         <v>110</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -6020,10 +6020,10 @@
         <v>110</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -6035,10 +6035,10 @@
         <v>110</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -6050,10 +6050,10 @@
         <v>110</v>
       </c>
       <c r="D23" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="E23" s="9" t="s">
         <v>715</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>716</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -6065,10 +6065,10 @@
         <v>110</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>718</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -6080,10 +6080,10 @@
         <v>110</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>725</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -6095,10 +6095,10 @@
         <v>110</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="E26" s="9" t="s">
         <v>720</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -6110,10 +6110,10 @@
         <v>110</v>
       </c>
       <c r="D27" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>722</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>723</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -6158,7 +6158,7 @@
         <v>130</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -6173,7 +6173,7 @@
         <v>121</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -6203,7 +6203,7 @@
         <v>135</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -6218,7 +6218,7 @@
         <v>88</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -6383,7 +6383,7 @@
         <v>83</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -6413,7 +6413,7 @@
         <v>100</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -6443,7 +6443,7 @@
         <v>127</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -6458,7 +6458,7 @@
         <v>98</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -6470,10 +6470,10 @@
         <v>138</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -6488,7 +6488,7 @@
         <v>99</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -6503,7 +6503,7 @@
         <v>97</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -6538,8 +6538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B44446-4EFF-1748-B076-59F83F2A5201}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6549,10 +6549,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
         <v>167</v>
-      </c>
-      <c r="B1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -6592,7 +6592,7 @@
         <v>146</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>733</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -6600,7 +6600,7 @@
         <v>147</v>
       </c>
       <c r="B7" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -6616,15 +6616,15 @@
         <v>150</v>
       </c>
       <c r="B9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B10" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -6695,10 +6695,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
         <v>167</v>
-      </c>
-      <c r="B1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -6706,7 +6706,7 @@
         <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
   </sheetData>
@@ -6726,12 +6726,12 @@
   <sheetData>
     <row r="1" spans="1:2" ht="22" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -6739,12 +6739,12 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -6752,54 +6752,54 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>193</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>195</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>197</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>199</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -6807,113 +6807,113 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="15"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="18" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="15" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="15" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="18"/>
+      <c r="B20" s="16" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="16" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="18"/>
+      <c r="B21" s="15" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="15" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="15" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="18"/>
+      <c r="B23" s="15" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="15" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
+      <c r="B24" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="B24" s="15" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="18"/>
+      <c r="B25" s="15" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="17"/>
-      <c r="B25" s="15" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>207</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>214</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="18" t="s">
-        <v>214</v>
+      <c r="A31" s="19" t="s">
+        <v>213</v>
       </c>
       <c r="B31" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="19"/>
+      <c r="B32" s="15" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="18"/>
-      <c r="B32" s="15" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -6921,32 +6921,32 @@
     </row>
     <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -6954,217 +6954,217 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>226</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>231</v>
+        <v>227</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="B43" s="18"/>
+        <v>228</v>
+      </c>
+      <c r="B43" s="19"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="B44" s="18"/>
+        <v>229</v>
+      </c>
+      <c r="B44" s="19"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="15"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="15"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
-        <v>214</v>
+      <c r="A50" s="18" t="s">
+        <v>213</v>
       </c>
       <c r="B50" s="16" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="18"/>
+      <c r="B51" s="15" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="17"/>
-      <c r="B51" s="15" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="18"/>
+      <c r="B52" s="15" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
-      <c r="B52" s="15" t="s">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="18"/>
+      <c r="B53" s="15" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
-      <c r="B53" s="15" t="s">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="18"/>
+      <c r="B54" s="15" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="15" t="s">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="18"/>
+      <c r="B55" s="15" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="15" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="18"/>
+      <c r="B56" s="15" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="15" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="B59" s="15" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="B59" s="15" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="18"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="18"/>
+      <c r="B61" s="15" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="17"/>
-      <c r="B61" s="15" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="15"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
-        <v>214</v>
+      <c r="A70" s="18" t="s">
+        <v>213</v>
       </c>
       <c r="B70" s="15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="18"/>
+      <c r="B71" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="18"/>
+      <c r="B72" s="15" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="17"/>
-      <c r="B71" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="17"/>
-      <c r="B72" s="15" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="18"/>
+      <c r="B73" s="15" t="s">
         <v>256</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="17"/>
-      <c r="B73" s="15" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -7172,82 +7172,82 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -7255,20 +7255,20 @@
     </row>
     <row r="91" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
@@ -7276,68 +7276,68 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="B95" s="16" t="s">
         <v>275</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="B96" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="B96" s="15" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="18" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="17" t="s">
+      <c r="B97" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="B97" s="15" t="s">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="18"/>
+      <c r="B98" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="18"/>
+      <c r="B99" s="15" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="17"/>
-      <c r="B98" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="17"/>
-      <c r="B99" s="15" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="18"/>
+      <c r="B100" s="15" t="s">
         <v>281</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="17"/>
-      <c r="B100" s="15" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="16" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B103" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
@@ -7345,10 +7345,10 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -7356,7 +7356,7 @@
     </row>
     <row r="107" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
@@ -7364,58 +7364,58 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="17" t="s">
         <v>287</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="19" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="15"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="17" t="s">
-        <v>207</v>
+      <c r="A112" s="18" t="s">
+        <v>206</v>
       </c>
       <c r="B112" s="15" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="18"/>
+      <c r="B113" s="15" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="17"/>
-      <c r="B113" s="15" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="15"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="17" t="s">
-        <v>214</v>
+      <c r="A115" s="18" t="s">
+        <v>213</v>
       </c>
       <c r="B115" s="15" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="18"/>
+      <c r="B116" s="15" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="17"/>
-      <c r="B116" s="15" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="18"/>
+      <c r="B117" s="15" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="17"/>
-      <c r="B117" s="15" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="18"/>
+      <c r="B118" s="15" t="s">
         <v>293</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="17"/>
-      <c r="B118" s="15" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -7423,7 +7423,7 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -7431,1946 +7431,1946 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="16" t="s">
+        <v>295</v>
+      </c>
+      <c r="B122" s="16" t="s">
         <v>296</v>
       </c>
-      <c r="B122" s="16" t="s">
+      <c r="C122" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="C122" s="16" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="17" t="s">
+      <c r="B123" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="B123" s="15" t="s">
+      <c r="C123" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="18"/>
+      <c r="B124" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="C123" s="18" t="s">
+      <c r="C124" s="19"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="18" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="17"/>
-      <c r="B124" s="19" t="s">
-        <v>300</v>
-      </c>
-      <c r="C124" s="18"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="17" t="s">
+      <c r="B125" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="B125" s="15" t="s">
+      <c r="C125" s="19" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="18"/>
+      <c r="B126" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="C125" s="18" t="s">
+      <c r="C126" s="19"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="18" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="17"/>
-      <c r="B126" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="C126" s="18"/>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="17" t="s">
+      <c r="B127" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="B127" s="15" t="s">
+      <c r="C127" s="19" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="18"/>
+      <c r="B128" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="C127" s="18" t="s">
+      <c r="C128" s="19"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="18" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="17"/>
-      <c r="B128" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="C128" s="18"/>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" s="17" t="s">
+      <c r="B129" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="B129" s="15" t="s">
+      <c r="C129" s="15" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="18"/>
+      <c r="B130" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="C129" s="15" t="s">
+      <c r="C130" s="15" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="17"/>
-      <c r="B130" s="15" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="18"/>
+      <c r="B131" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="C130" s="15" t="s">
+      <c r="C131" s="15" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="17"/>
-      <c r="B131" s="15" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="18"/>
+      <c r="B132" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C132" s="15" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="17"/>
-      <c r="B132" s="15" t="s">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="18"/>
+      <c r="B133" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="C132" s="15" t="s">
+      <c r="C133" s="15" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="17"/>
-      <c r="B133" s="15" t="s">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="18"/>
+      <c r="B134" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="C133" s="15" t="s">
+      <c r="C134" s="15" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="17"/>
-      <c r="B134" s="15" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="18"/>
+      <c r="B135" s="15"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="18"/>
+      <c r="B136" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="C134" s="15" t="s">
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="18" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="17"/>
-      <c r="B135" s="15"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="17"/>
-      <c r="B136" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="17" t="s">
+      <c r="B137" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="B137" s="15" t="s">
+      <c r="C137" s="15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="18"/>
+      <c r="B138" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="C137" s="15" t="s">
+      <c r="C138" s="15" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="17"/>
-      <c r="B138" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="C138" s="15" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="18" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A139" s="17" t="s">
+      <c r="B139" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="B139" s="15" t="s">
+      <c r="C139" s="15" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="18"/>
+      <c r="B140" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="C139" s="15" t="s">
+      <c r="C140" s="15" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A140" s="17"/>
-      <c r="B140" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="C140" s="15" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="18" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A141" s="17" t="s">
+      <c r="B141" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="B141" s="15" t="s">
+      <c r="C141" s="15" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="18"/>
+      <c r="B142" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="C141" s="15" t="s">
+      <c r="C142" s="15" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" s="17"/>
-      <c r="B142" s="15" t="s">
-        <v>336</v>
-      </c>
-      <c r="C142" s="15" t="s">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="18" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" s="17" t="s">
+      <c r="B143" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="B143" s="15" t="s">
+      <c r="C143" s="15" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="18"/>
+      <c r="B144" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="C143" s="15" t="s">
+      <c r="C144" s="15" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A144" s="17"/>
-      <c r="B144" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="C144" s="15" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="18"/>
+      <c r="C145" s="15" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145" s="17"/>
-      <c r="C145" s="15" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="18" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A146" s="17" t="s">
+      <c r="B146" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="B146" s="15" t="s">
+      <c r="C146" s="19" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="18"/>
+      <c r="B147" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="C146" s="18" t="s">
+      <c r="C147" s="19"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="18" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A147" s="17"/>
-      <c r="B147" s="15" t="s">
-        <v>347</v>
-      </c>
-      <c r="C147" s="18"/>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A148" s="17" t="s">
+      <c r="B148" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="B148" s="15" t="s">
+      <c r="C148" s="15" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="18"/>
+      <c r="B149" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="C148" s="15" t="s">
+      <c r="C149" s="15" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A149" s="17"/>
-      <c r="B149" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="C149" s="15" t="s">
-        <v>360</v>
-      </c>
-    </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A150" s="17"/>
+      <c r="A150" s="18"/>
       <c r="B150" s="15"/>
       <c r="C150" s="15" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="18"/>
+      <c r="B151" s="15" t="s">
+        <v>351</v>
+      </c>
+      <c r="C151" s="15" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A151" s="17"/>
-      <c r="B151" s="15" t="s">
-        <v>352</v>
-      </c>
-      <c r="C151" s="15" t="s">
-        <v>362</v>
-      </c>
-    </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A152" s="17"/>
+      <c r="A152" s="18"/>
       <c r="B152" s="15"/>
       <c r="C152" s="15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="18"/>
+      <c r="B153" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C153" s="15" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A153" s="17"/>
-      <c r="B153" s="15" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="18"/>
+      <c r="B154" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C153" s="15" t="s">
+      <c r="C154" s="15" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A154" s="17"/>
-      <c r="B154" s="15" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="18"/>
+      <c r="B155" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="C154" s="15" t="s">
+      <c r="C155" s="15" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A155" s="17"/>
-      <c r="B155" s="15" t="s">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="18"/>
+      <c r="B156" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="C155" s="15" t="s">
+      <c r="C156" s="15" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A156" s="17"/>
-      <c r="B156" s="15" t="s">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="18"/>
+      <c r="B157" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C156" s="15" t="s">
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="18"/>
+      <c r="B158" s="15"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="18"/>
+      <c r="B159" s="16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="18"/>
+      <c r="B160" s="15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="18" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A157" s="17"/>
-      <c r="B157" s="15" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A158" s="17"/>
-      <c r="B158" s="15"/>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A159" s="17"/>
-      <c r="B159" s="16" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A160" s="17"/>
-      <c r="B160" s="15" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" s="17" t="s">
+      <c r="B161" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="B161" s="15" t="s">
+      <c r="C161" s="15" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="18"/>
+      <c r="B162" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="C161" s="15" t="s">
+      <c r="C162" s="15" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" s="17"/>
-      <c r="B162" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="C162" s="15" t="s">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="18"/>
+      <c r="B163" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="C163" s="15" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" s="17"/>
-      <c r="B163" s="15" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="18"/>
+      <c r="B164" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="C163" s="15" t="s">
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="18" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" s="17"/>
-      <c r="B164" s="15" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" s="17" t="s">
+      <c r="B165" s="19" t="s">
         <v>374</v>
       </c>
-      <c r="B165" s="18" t="s">
+      <c r="C165" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="C165" s="15" t="s">
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="18"/>
+      <c r="B166" s="19"/>
+      <c r="C166" s="15" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" s="17"/>
-      <c r="B166" s="18"/>
-      <c r="C166" s="15" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="18"/>
+      <c r="B167" s="19"/>
+      <c r="C167" s="15" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A167" s="17"/>
-      <c r="B167" s="18"/>
-      <c r="C167" s="15" t="s">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="18"/>
+      <c r="B168" s="19"/>
+      <c r="C168" s="15" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" s="17"/>
-      <c r="B168" s="18"/>
-      <c r="C168" s="15" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="18"/>
+      <c r="B169" s="19"/>
+      <c r="C169" s="15" t="s">
         <v>379</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A169" s="17"/>
-      <c r="B169" s="18"/>
-      <c r="C169" s="15" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="B170" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="B170" s="15" t="s">
+      <c r="C170" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="C170" s="15" t="s">
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="18" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A171" s="17" t="s">
+      <c r="B171" s="15" t="s">
         <v>384</v>
       </c>
-      <c r="B171" s="15" t="s">
+      <c r="C171" s="19" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="18"/>
+      <c r="B172" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="C171" s="18" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172" s="17"/>
-      <c r="B172" s="15" t="s">
-        <v>386</v>
-      </c>
-      <c r="C172" s="18"/>
+      <c r="C172" s="19"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="B173" s="15" t="s">
         <v>388</v>
       </c>
-      <c r="B173" s="15" t="s">
+      <c r="C173" s="15" t="s">
         <v>389</v>
       </c>
-      <c r="C173" s="15" t="s">
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="18" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A174" s="17" t="s">
+      <c r="B174" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="B174" s="15" t="s">
+      <c r="C174" s="19" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="18"/>
+      <c r="B175" s="15" t="s">
         <v>392</v>
       </c>
-      <c r="C174" s="18" t="s">
+      <c r="C175" s="19"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="18" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" s="17"/>
-      <c r="B175" s="15" t="s">
-        <v>393</v>
-      </c>
-      <c r="C175" s="18"/>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176" s="17" t="s">
+      <c r="B176" s="15" t="s">
         <v>395</v>
       </c>
-      <c r="B176" s="15" t="s">
+      <c r="C176" s="19" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="18"/>
+      <c r="B177" s="15" t="s">
         <v>396</v>
       </c>
-      <c r="C176" s="18" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="17"/>
-      <c r="B177" s="15" t="s">
-        <v>397</v>
-      </c>
-      <c r="C177" s="18"/>
+      <c r="C177" s="19"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="B178" s="15" t="s">
         <v>399</v>
       </c>
-      <c r="B178" s="15" t="s">
+      <c r="C178" s="15" t="s">
         <v>400</v>
-      </c>
-      <c r="C178" s="15" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="B179" s="15" t="s">
         <v>402</v>
       </c>
-      <c r="B179" s="15" t="s">
+      <c r="C179" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="C179" s="15" t="s">
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="18" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180" s="17" t="s">
+      <c r="B180" s="15" t="s">
         <v>405</v>
       </c>
-      <c r="B180" s="15" t="s">
+      <c r="C180" s="15" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="18"/>
+      <c r="B181" s="15" t="s">
         <v>406</v>
       </c>
-      <c r="C180" s="15" t="s">
+      <c r="C181" s="15" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" s="17"/>
-      <c r="B181" s="15" t="s">
-        <v>407</v>
-      </c>
-      <c r="C181" s="15" t="s">
+    <row r="182" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A182" s="18" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A182" s="17" t="s">
+      <c r="B182" s="19" t="s">
         <v>410</v>
       </c>
-      <c r="B182" s="18" t="s">
+      <c r="C182" s="14" t="s">
         <v>411</v>
       </c>
-      <c r="C182" s="14" t="s">
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="18"/>
+      <c r="B183" s="19"/>
+      <c r="C183" s="15" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A183" s="17"/>
-      <c r="B183" s="18"/>
-      <c r="C183" s="15" t="s">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="18" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184" s="17" t="s">
+      <c r="B184" s="19" t="s">
         <v>414</v>
       </c>
-      <c r="B184" s="18" t="s">
+      <c r="C184" s="15" t="s">
         <v>415</v>
       </c>
-      <c r="C184" s="15" t="s">
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="18"/>
+      <c r="B185" s="19"/>
+      <c r="C185" s="15" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="18" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" s="17"/>
-      <c r="B185" s="18"/>
-      <c r="C185" s="15" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A186" s="17" t="s">
+      <c r="B186" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="B186" s="18" t="s">
+      <c r="C186" s="15" t="s">
         <v>418</v>
       </c>
-      <c r="C186" s="15" t="s">
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="18"/>
+      <c r="B187" s="19"/>
+      <c r="C187" s="15" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A187" s="17"/>
-      <c r="B187" s="18"/>
-      <c r="C187" s="15" t="s">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="18"/>
+      <c r="B188" s="19"/>
+      <c r="C188" s="15" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A188" s="17"/>
-      <c r="B188" s="18"/>
-      <c r="C188" s="15" t="s">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="18" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189" s="17" t="s">
+      <c r="B189" s="15" t="s">
         <v>422</v>
       </c>
-      <c r="B189" s="15" t="s">
+      <c r="C189" s="19" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="18"/>
+      <c r="B190" s="15" t="s">
         <v>423</v>
       </c>
-      <c r="C189" s="18" t="s">
+      <c r="C190" s="19"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="18" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A190" s="17"/>
-      <c r="B190" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C190" s="18"/>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A191" s="17" t="s">
+      <c r="B191" s="15" t="s">
         <v>426</v>
       </c>
-      <c r="B191" s="15" t="s">
+      <c r="C191" s="19" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="18"/>
+      <c r="B192" s="15" t="s">
         <v>427</v>
       </c>
-      <c r="C191" s="18" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A192" s="17"/>
-      <c r="B192" s="15" t="s">
-        <v>428</v>
-      </c>
-      <c r="C192" s="18"/>
+      <c r="C192" s="19"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="16" t="s">
+        <v>429</v>
+      </c>
+      <c r="B193" s="15" t="s">
         <v>430</v>
       </c>
-      <c r="B193" s="15" t="s">
+      <c r="C193" s="15" t="s">
         <v>431</v>
       </c>
-      <c r="C193" s="15" t="s">
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="18" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194" s="17" t="s">
+      <c r="B194" s="15" t="s">
         <v>433</v>
       </c>
-      <c r="B194" s="15" t="s">
+      <c r="C194" s="19" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="18"/>
+      <c r="B195" s="15" t="s">
         <v>434</v>
       </c>
-      <c r="C194" s="18" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" s="17"/>
-      <c r="B195" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="C195" s="18"/>
+      <c r="C195" s="19"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="16" t="s">
+        <v>436</v>
+      </c>
+      <c r="B196" s="15" t="s">
         <v>437</v>
       </c>
-      <c r="B196" s="15" t="s">
+      <c r="C196" s="15" t="s">
         <v>438</v>
       </c>
-      <c r="C196" s="15" t="s">
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="18" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" s="17" t="s">
+      <c r="B197" s="15" t="s">
         <v>440</v>
       </c>
-      <c r="B197" s="15" t="s">
+      <c r="C197" s="19" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="18"/>
+      <c r="B198" s="15" t="s">
         <v>441</v>
       </c>
-      <c r="C197" s="18" t="s">
+      <c r="C198" s="19"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="18" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" s="17"/>
-      <c r="B198" s="15" t="s">
-        <v>442</v>
-      </c>
-      <c r="C198" s="18"/>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" s="17" t="s">
+      <c r="B199" s="15" t="s">
         <v>444</v>
       </c>
-      <c r="B199" s="15" t="s">
+      <c r="C199" s="19" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="18"/>
+      <c r="B200" s="17" t="s">
         <v>445</v>
       </c>
-      <c r="C199" s="18" t="s">
+      <c r="C200" s="19"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="18"/>
+      <c r="B201" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="C201" s="19"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" s="18" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" s="17"/>
-      <c r="B200" s="19" t="s">
-        <v>446</v>
-      </c>
-      <c r="C200" s="18"/>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" s="17"/>
-      <c r="B201" s="15" t="s">
-        <v>447</v>
-      </c>
-      <c r="C201" s="18"/>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A202" s="17" t="s">
+      <c r="B202" s="15" t="s">
         <v>449</v>
       </c>
-      <c r="B202" s="15" t="s">
+      <c r="C202" s="19" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" s="18"/>
+      <c r="B203" s="15" t="s">
         <v>450</v>
       </c>
-      <c r="C202" s="18" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A203" s="17"/>
-      <c r="B203" s="15" t="s">
-        <v>451</v>
-      </c>
-      <c r="C203" s="18"/>
+      <c r="C203" s="19"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="16" t="s">
+        <v>452</v>
+      </c>
+      <c r="B204" s="15" t="s">
         <v>453</v>
       </c>
-      <c r="B204" s="15" t="s">
+      <c r="C204" s="15" t="s">
         <v>454</v>
-      </c>
-      <c r="C204" s="15" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="16" t="s">
+        <v>455</v>
+      </c>
+      <c r="B205" s="15" t="s">
         <v>456</v>
       </c>
-      <c r="B205" s="15" t="s">
+      <c r="C205" s="15" t="s">
         <v>457</v>
-      </c>
-      <c r="C205" s="15" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="16" t="s">
+        <v>458</v>
+      </c>
+      <c r="B206" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="B206" s="15" t="s">
+      <c r="C206" s="15" t="s">
         <v>460</v>
       </c>
-      <c r="C206" s="15" t="s">
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" s="18" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A207" s="17" t="s">
+      <c r="B207" s="15" t="s">
         <v>462</v>
       </c>
-      <c r="B207" s="15" t="s">
+      <c r="C207" s="19" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="18"/>
+      <c r="B208" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="C207" s="18" t="s">
+      <c r="C208" s="19"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" s="18" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208" s="17"/>
-      <c r="B208" s="15" t="s">
-        <v>464</v>
-      </c>
-      <c r="C208" s="18"/>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A209" s="17" t="s">
+      <c r="B209" s="15" t="s">
         <v>466</v>
       </c>
-      <c r="B209" s="15" t="s">
+      <c r="C209" s="19" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" s="18"/>
+      <c r="B210" s="15" t="s">
         <v>467</v>
       </c>
-      <c r="C209" s="18" t="s">
+      <c r="C210" s="19"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" s="18" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A210" s="17"/>
-      <c r="B210" s="15" t="s">
-        <v>468</v>
-      </c>
-      <c r="C210" s="18"/>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A211" s="17" t="s">
+      <c r="B211" s="15" t="s">
         <v>470</v>
       </c>
-      <c r="B211" s="15" t="s">
+      <c r="C211" s="15" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" s="18"/>
+      <c r="B212" s="15" t="s">
         <v>471</v>
       </c>
-      <c r="C211" s="15" t="s">
+      <c r="C212" s="17" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A212" s="17"/>
-      <c r="B212" s="15" t="s">
-        <v>472</v>
-      </c>
-      <c r="C212" s="19" t="s">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" s="18" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A213" s="17" t="s">
+      <c r="B213" s="15" t="s">
         <v>475</v>
       </c>
-      <c r="B213" s="15" t="s">
+      <c r="C213" s="19" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" s="18"/>
+      <c r="B214" s="15" t="s">
         <v>476</v>
       </c>
-      <c r="C213" s="18" t="s">
+      <c r="C214" s="19"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" s="18" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A214" s="17"/>
-      <c r="B214" s="15" t="s">
-        <v>477</v>
-      </c>
-      <c r="C214" s="18"/>
-    </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A215" s="17" t="s">
+      <c r="B215" s="15" t="s">
         <v>479</v>
       </c>
-      <c r="B215" s="15" t="s">
+      <c r="C215" s="19" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" s="18"/>
+      <c r="B216" s="15" t="s">
         <v>480</v>
       </c>
-      <c r="C215" s="18" t="s">
+      <c r="C216" s="19"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" s="18" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A216" s="17"/>
-      <c r="B216" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="C216" s="18"/>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A217" s="17" t="s">
+      <c r="B217" s="15" t="s">
         <v>483</v>
       </c>
-      <c r="B217" s="15" t="s">
+      <c r="C217" s="19" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" s="18"/>
+      <c r="B218" s="15" t="s">
         <v>484</v>
       </c>
-      <c r="C217" s="18" t="s">
+      <c r="C218" s="19"/>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" s="18" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A218" s="17"/>
-      <c r="B218" s="15" t="s">
-        <v>485</v>
-      </c>
-      <c r="C218" s="18"/>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A219" s="17" t="s">
+      <c r="B219" s="15" t="s">
         <v>487</v>
       </c>
-      <c r="B219" s="15" t="s">
+      <c r="C219" s="19" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" s="18"/>
+      <c r="B220" s="15" t="s">
         <v>488</v>
       </c>
-      <c r="C219" s="18" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A220" s="17"/>
-      <c r="B220" s="15" t="s">
-        <v>489</v>
-      </c>
-      <c r="C220" s="18"/>
+      <c r="C220" s="19"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="16" t="s">
+        <v>490</v>
+      </c>
+      <c r="B221" s="15" t="s">
         <v>491</v>
       </c>
-      <c r="B221" s="15" t="s">
+      <c r="C221" s="15" t="s">
         <v>492</v>
       </c>
-      <c r="C221" s="15" t="s">
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" s="18" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A222" s="17" t="s">
+      <c r="B222" s="19" t="s">
         <v>494</v>
       </c>
-      <c r="B222" s="18" t="s">
+      <c r="C222" s="15" t="s">
         <v>495</v>
       </c>
-      <c r="C222" s="15" t="s">
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" s="18"/>
+      <c r="B223" s="19"/>
+      <c r="C223" s="15" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A223" s="17"/>
-      <c r="B223" s="18"/>
-      <c r="C223" s="15" t="s">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" s="18" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A224" s="17" t="s">
+      <c r="B224" s="19" t="s">
         <v>498</v>
       </c>
-      <c r="B224" s="18" t="s">
+      <c r="C224" s="15" t="s">
         <v>499</v>
       </c>
-      <c r="C224" s="15" t="s">
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" s="18"/>
+      <c r="B225" s="19"/>
+      <c r="C225" s="15" t="s">
         <v>500</v>
       </c>
     </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A225" s="17"/>
-      <c r="B225" s="18"/>
-      <c r="C225" s="15" t="s">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" s="18"/>
+      <c r="B226" s="19"/>
+      <c r="C226" s="15" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A226" s="17"/>
-      <c r="B226" s="18"/>
-      <c r="C226" s="15" t="s">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" s="18" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A227" s="17" t="s">
+      <c r="B227" s="19" t="s">
         <v>503</v>
       </c>
-      <c r="B227" s="18" t="s">
+      <c r="C227" s="15" t="s">
         <v>504</v>
       </c>
-      <c r="C227" s="15" t="s">
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" s="18"/>
+      <c r="B228" s="19"/>
+      <c r="C228" s="15" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" s="18"/>
+      <c r="B229" s="19"/>
+      <c r="C229" s="15" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" s="18" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A228" s="17"/>
-      <c r="B228" s="18"/>
-      <c r="C228" s="15" t="s">
+      <c r="B230" s="15" t="s">
+        <v>506</v>
+      </c>
+      <c r="C230" s="15" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" s="18"/>
+      <c r="B231" s="15" t="s">
+        <v>507</v>
+      </c>
+      <c r="C231" s="15" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" s="18"/>
+      <c r="C232" s="15" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" s="18"/>
+      <c r="C233" s="15" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" s="18"/>
+      <c r="C234" s="15" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A229" s="17"/>
-      <c r="B229" s="18"/>
-      <c r="C229" s="15" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A230" s="17" t="s">
-        <v>506</v>
-      </c>
-      <c r="B230" s="15" t="s">
-        <v>507</v>
-      </c>
-      <c r="C230" s="15" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A231" s="17"/>
-      <c r="B231" s="15" t="s">
-        <v>508</v>
-      </c>
-      <c r="C231" s="15" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A232" s="17"/>
-      <c r="C232" s="15" t="s">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" s="18" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A233" s="17"/>
-      <c r="C233" s="15" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A234" s="17"/>
-      <c r="C234" s="15" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A235" s="17" t="s">
+      <c r="B235" s="15" t="s">
         <v>512</v>
       </c>
-      <c r="B235" s="15" t="s">
+      <c r="C235" s="19" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" s="18"/>
+      <c r="B236" s="15" t="s">
         <v>513</v>
       </c>
-      <c r="C235" s="18" t="s">
+      <c r="C236" s="19"/>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" s="18" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A236" s="17"/>
-      <c r="B236" s="15" t="s">
-        <v>514</v>
-      </c>
-      <c r="C236" s="18"/>
-    </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A237" s="17" t="s">
+      <c r="B237" s="15" t="s">
         <v>516</v>
       </c>
-      <c r="B237" s="15" t="s">
+      <c r="C237" s="19" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" s="18"/>
+      <c r="B238" s="15" t="s">
         <v>517</v>
       </c>
-      <c r="C237" s="18" t="s">
+      <c r="C238" s="19"/>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" s="18" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A238" s="17"/>
-      <c r="B238" s="15" t="s">
-        <v>518</v>
-      </c>
-      <c r="C238" s="18"/>
-    </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A239" s="17" t="s">
+      <c r="B239" s="15" t="s">
         <v>520</v>
       </c>
-      <c r="B239" s="15" t="s">
+      <c r="C239" s="15" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" s="18"/>
+      <c r="B240" s="15" t="s">
         <v>521</v>
       </c>
-      <c r="C239" s="15" t="s">
+      <c r="C240" s="15" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A240" s="17"/>
-      <c r="B240" s="15" t="s">
-        <v>522</v>
-      </c>
-      <c r="C240" s="15" t="s">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" s="18"/>
+      <c r="C241" s="15" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A241" s="17"/>
-      <c r="C241" s="15" t="s">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" s="18" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A242" s="17" t="s">
+      <c r="B242" s="15" t="s">
         <v>526</v>
       </c>
-      <c r="B242" s="15" t="s">
+      <c r="C242" s="15" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" s="18"/>
+      <c r="B243" s="15" t="s">
         <v>527</v>
       </c>
-      <c r="C242" s="15" t="s">
+      <c r="C243" s="15" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A243" s="17"/>
-      <c r="B243" s="15" t="s">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" s="18"/>
+      <c r="B244" s="15" t="s">
         <v>528</v>
       </c>
-      <c r="C243" s="15" t="s">
+      <c r="C244" s="15" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A244" s="17"/>
-      <c r="B244" s="15" t="s">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" s="18"/>
+      <c r="B245" s="15" t="s">
         <v>529</v>
       </c>
-      <c r="C244" s="15" t="s">
+      <c r="C245" s="15" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A245" s="17"/>
-      <c r="B245" s="15" t="s">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" s="18"/>
+      <c r="B246" s="15" t="s">
         <v>530</v>
       </c>
-      <c r="C245" s="15" t="s">
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A247" s="18"/>
+      <c r="B247" s="15" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A248" s="18"/>
+      <c r="B248" s="15" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A249" s="18"/>
+      <c r="B249" s="15" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A250" s="18" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A246" s="17"/>
-      <c r="B246" s="15" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A247" s="17"/>
-      <c r="B247" s="15" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A248" s="17"/>
-      <c r="B248" s="15" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A249" s="17"/>
-      <c r="B249" s="15" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A250" s="17" t="s">
+      <c r="B250" s="15" t="s">
         <v>539</v>
       </c>
-      <c r="B250" s="15" t="s">
+      <c r="C250" s="19" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A251" s="18"/>
+      <c r="B251" s="15" t="s">
         <v>540</v>
       </c>
-      <c r="C250" s="18" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A251" s="17"/>
-      <c r="B251" s="15" t="s">
+      <c r="C251" s="19"/>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A252" s="18"/>
+      <c r="B252" s="15" t="s">
         <v>541</v>
       </c>
-      <c r="C251" s="18"/>
-    </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A252" s="17"/>
-      <c r="B252" s="15" t="s">
+      <c r="C252" s="19"/>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A253" s="18"/>
+      <c r="B253" s="15" t="s">
         <v>542</v>
       </c>
-      <c r="C252" s="18"/>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A253" s="17"/>
-      <c r="B253" s="15" t="s">
-        <v>543</v>
-      </c>
-      <c r="C253" s="18"/>
+      <c r="C253" s="19"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="16" t="s">
+        <v>544</v>
+      </c>
+      <c r="B254" s="15" t="s">
         <v>545</v>
       </c>
-      <c r="B254" s="15" t="s">
+      <c r="C254" s="15" t="s">
         <v>546</v>
-      </c>
-      <c r="C254" s="15" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="B255" s="15" t="s">
         <v>548</v>
       </c>
-      <c r="B255" s="15" t="s">
+      <c r="C255" s="15" t="s">
         <v>549</v>
       </c>
-      <c r="C255" s="15" t="s">
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A256" s="18" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A256" s="17" t="s">
+      <c r="B256" s="15" t="s">
         <v>551</v>
       </c>
-      <c r="B256" s="15" t="s">
+      <c r="C256" s="19" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A257" s="18"/>
+      <c r="B257" s="15" t="s">
         <v>552</v>
       </c>
-      <c r="C256" s="18" t="s">
+      <c r="C257" s="19"/>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A258" s="18" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A257" s="17"/>
-      <c r="B257" s="15" t="s">
-        <v>553</v>
-      </c>
-      <c r="C257" s="18"/>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A258" s="17" t="s">
+      <c r="B258" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C258" s="15" t="s">
         <v>555</v>
       </c>
-      <c r="B258" s="15" t="s">
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A259" s="18"/>
+      <c r="B259" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="C258" s="15" t="s">
+      <c r="C259" s="15" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A260" s="18"/>
+      <c r="C260" s="15" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A259" s="17"/>
-      <c r="B259" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="C259" s="15" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A260" s="17"/>
-      <c r="C260" s="15" t="s">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A261" s="18" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="261" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A261" s="17" t="s">
+      <c r="B261" s="19" t="s">
         <v>558</v>
       </c>
-      <c r="B261" s="18" t="s">
+      <c r="C261" s="15" t="s">
         <v>559</v>
       </c>
-      <c r="C261" s="15" t="s">
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A262" s="18"/>
+      <c r="B262" s="19"/>
+      <c r="C262" s="15" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="262" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A262" s="17"/>
-      <c r="B262" s="18"/>
-      <c r="C262" s="15" t="s">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A263" s="18"/>
+      <c r="B263" s="19"/>
+      <c r="C263" s="15" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="263" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A263" s="17"/>
-      <c r="B263" s="18"/>
-      <c r="C263" s="15" t="s">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A264" s="18" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="264" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A264" s="17" t="s">
+      <c r="B264" s="19" t="s">
         <v>563</v>
       </c>
-      <c r="B264" s="18" t="s">
+      <c r="C264" s="15" t="s">
         <v>564</v>
       </c>
-      <c r="C264" s="15" t="s">
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A265" s="18"/>
+      <c r="B265" s="19"/>
+      <c r="C265" s="15" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="265" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A265" s="17"/>
-      <c r="B265" s="18"/>
-      <c r="C265" s="15" t="s">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A266" s="18"/>
+      <c r="B266" s="19"/>
+      <c r="C266" s="15" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="266" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A266" s="17"/>
-      <c r="B266" s="18"/>
-      <c r="C266" s="15" t="s">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A267" s="18" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="267" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A267" s="17" t="s">
+      <c r="B267" s="15" t="s">
         <v>568</v>
       </c>
-      <c r="B267" s="15" t="s">
+      <c r="C267" s="19" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A268" s="18"/>
+      <c r="B268" s="15" t="s">
         <v>569</v>
       </c>
-      <c r="C267" s="18" t="s">
+      <c r="C268" s="19"/>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A269" s="18" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="268" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A268" s="17"/>
-      <c r="B268" s="15" t="s">
-        <v>570</v>
-      </c>
-      <c r="C268" s="18"/>
-    </row>
-    <row r="269" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A269" s="17" t="s">
+      <c r="B269" s="15" t="s">
         <v>572</v>
       </c>
-      <c r="B269" s="15" t="s">
+      <c r="C269" s="19" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A270" s="18"/>
+      <c r="B270" s="15" t="s">
         <v>573</v>
       </c>
-      <c r="C269" s="18" t="s">
+      <c r="C270" s="19"/>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A271" s="18" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="270" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A270" s="17"/>
-      <c r="B270" s="15" t="s">
-        <v>574</v>
-      </c>
-      <c r="C270" s="18"/>
-    </row>
-    <row r="271" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A271" s="17" t="s">
+      <c r="B271" s="15" t="s">
         <v>576</v>
       </c>
-      <c r="B271" s="15" t="s">
+      <c r="C271" s="15" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A272" s="18"/>
+      <c r="B272" s="15" t="s">
         <v>577</v>
       </c>
-      <c r="C271" s="15" t="s">
+      <c r="C272" s="15" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="272" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A272" s="17"/>
-      <c r="B272" s="15" t="s">
-        <v>578</v>
-      </c>
-      <c r="C272" s="15" t="s">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A273" s="18"/>
+      <c r="C273" s="15" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A273" s="17"/>
-      <c r="C273" s="15" t="s">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A274" s="18"/>
+      <c r="C274" s="15" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A274" s="17"/>
-      <c r="C274" s="15" t="s">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A275" s="18" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A275" s="17" t="s">
+      <c r="B275" s="15" t="s">
         <v>583</v>
       </c>
-      <c r="B275" s="15" t="s">
+      <c r="C275" s="19" t="s">
         <v>584</v>
       </c>
-      <c r="C275" s="18" t="s">
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A276" s="18"/>
+      <c r="B276" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="C276" s="19"/>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A277" s="18" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A276" s="17"/>
-      <c r="B276" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C276" s="18"/>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A277" s="17" t="s">
+      <c r="B277" s="15" t="s">
         <v>586</v>
       </c>
-      <c r="B277" s="15" t="s">
+      <c r="C277" s="19" t="s">
         <v>587</v>
       </c>
-      <c r="C277" s="18" t="s">
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A278" s="18"/>
+      <c r="B278" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="C278" s="19"/>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A279" s="18" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A278" s="17"/>
-      <c r="B278" s="15" t="s">
-        <v>424</v>
-      </c>
-      <c r="C278" s="18"/>
-    </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A279" s="17" t="s">
+      <c r="B279" s="15" t="s">
         <v>589</v>
       </c>
-      <c r="B279" s="15" t="s">
+      <c r="C279" s="19" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A280" s="18"/>
+      <c r="B280" s="15" t="s">
         <v>590</v>
       </c>
-      <c r="C279" s="18" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A280" s="17"/>
-      <c r="B280" s="15" t="s">
-        <v>591</v>
-      </c>
-      <c r="C280" s="18"/>
+      <c r="C280" s="19"/>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="16" t="s">
+        <v>592</v>
+      </c>
+      <c r="B281" s="15" t="s">
         <v>593</v>
       </c>
-      <c r="B281" s="15" t="s">
+      <c r="C281" s="15" t="s">
         <v>594</v>
-      </c>
-      <c r="C281" s="15" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="16" t="s">
+        <v>595</v>
+      </c>
+      <c r="B282" s="15" t="s">
         <v>596</v>
       </c>
-      <c r="B282" s="15" t="s">
+      <c r="C282" s="15" t="s">
         <v>597</v>
-      </c>
-      <c r="C282" s="15" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="16" t="s">
+        <v>598</v>
+      </c>
+      <c r="B283" s="15" t="s">
         <v>599</v>
       </c>
-      <c r="B283" s="15" t="s">
+      <c r="C283" s="15" t="s">
         <v>600</v>
       </c>
-      <c r="C283" s="15" t="s">
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A284" s="18" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A284" s="17" t="s">
+      <c r="B284" s="15" t="s">
         <v>602</v>
       </c>
-      <c r="B284" s="15" t="s">
+      <c r="C284" s="19" t="s">
         <v>603</v>
       </c>
-      <c r="C284" s="18" t="s">
-        <v>604</v>
-      </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A285" s="17"/>
+      <c r="A285" s="18"/>
       <c r="B285" s="15" t="s">
-        <v>481</v>
-      </c>
-      <c r="C285" s="18"/>
+        <v>480</v>
+      </c>
+      <c r="C285" s="19"/>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="16" t="s">
+        <v>604</v>
+      </c>
+      <c r="B286" s="15" t="s">
         <v>605</v>
       </c>
-      <c r="B286" s="15" t="s">
+      <c r="C286" s="15" t="s">
         <v>606</v>
       </c>
-      <c r="C286" s="15" t="s">
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A287" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B287" s="15" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A287" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="B287" s="15" t="s">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A288" s="18"/>
+      <c r="B288" s="15" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A288" s="17"/>
-      <c r="B288" s="15" t="s">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B289" s="15" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A289" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="B289" s="15" t="s">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" s="18"/>
+      <c r="B290" s="15" t="s">
         <v>610</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A290" s="17"/>
-      <c r="B290" s="15" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B291" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B292" s="15" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" s="16" t="s">
+        <v>612</v>
+      </c>
+      <c r="B293" s="15" t="s">
         <v>613</v>
-      </c>
-      <c r="B293" s="15" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" s="16" t="s">
+        <v>614</v>
+      </c>
+      <c r="B294" s="15" t="s">
         <v>615</v>
-      </c>
-      <c r="B294" s="15" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" s="15" t="s">
+        <v>616</v>
+      </c>
+      <c r="B295" s="15" t="s">
         <v>617</v>
-      </c>
-      <c r="B295" s="15" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="B296" s="15" t="s">
         <v>619</v>
-      </c>
-      <c r="B296" s="15" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="B297" s="15" t="s">
         <v>621</v>
-      </c>
-      <c r="B297" s="15" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" s="16" t="s">
+        <v>622</v>
+      </c>
+      <c r="B298" s="15" t="s">
         <v>623</v>
-      </c>
-      <c r="B298" s="15" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" s="16" t="s">
+        <v>624</v>
+      </c>
+      <c r="B299" s="15" t="s">
         <v>625</v>
-      </c>
-      <c r="B299" s="15" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" s="16" t="s">
+        <v>626</v>
+      </c>
+      <c r="B300" s="15" t="s">
         <v>627</v>
-      </c>
-      <c r="B300" s="15" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" s="16" t="s">
+        <v>628</v>
+      </c>
+      <c r="B301" s="15" t="s">
         <v>629</v>
-      </c>
-      <c r="B301" s="15" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" s="16" t="s">
+        <v>630</v>
+      </c>
+      <c r="B302" s="15" t="s">
         <v>631</v>
-      </c>
-      <c r="B302" s="15" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" s="16" t="s">
+        <v>632</v>
+      </c>
+      <c r="B303" s="15" t="s">
         <v>633</v>
-      </c>
-      <c r="B303" s="15" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" s="16" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B304" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="B305" s="15" t="s">
         <v>636</v>
-      </c>
-      <c r="B305" s="15" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="B306" s="15" t="s">
         <v>638</v>
-      </c>
-      <c r="B306" s="15" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" s="16" t="s">
+        <v>639</v>
+      </c>
+      <c r="B307" s="15" t="s">
         <v>640</v>
       </c>
-      <c r="B307" s="15" t="s">
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B308" s="15" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A308" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="B308" s="15" t="s">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A309" s="18"/>
+      <c r="B309" s="15" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A309" s="17"/>
-      <c r="B309" s="15" t="s">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" s="18"/>
+      <c r="B310" s="15" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A310" s="17"/>
-      <c r="B310" s="15" t="s">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" s="18"/>
+      <c r="B311" s="15" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A311" s="17"/>
-      <c r="B311" s="15" t="s">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A312" s="18"/>
+      <c r="B312" s="15" t="s">
         <v>645</v>
-      </c>
-    </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A312" s="17"/>
-      <c r="B312" s="15" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B313" s="15" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B314" s="15" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" s="16" t="s">
+        <v>648</v>
+      </c>
+      <c r="B315" s="15" t="s">
         <v>649</v>
-      </c>
-      <c r="B315" s="15" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" s="16" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B316" s="15" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" s="16" t="s">
+        <v>651</v>
+      </c>
+      <c r="B317" s="15" t="s">
         <v>652</v>
-      </c>
-      <c r="B317" s="15" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" s="16" t="s">
+        <v>653</v>
+      </c>
+      <c r="B318" s="15" t="s">
         <v>654</v>
-      </c>
-      <c r="B318" s="15" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" s="16" t="s">
+        <v>655</v>
+      </c>
+      <c r="B319" s="15" t="s">
         <v>656</v>
-      </c>
-      <c r="B319" s="15" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" s="16" t="s">
+        <v>657</v>
+      </c>
+      <c r="B320" s="15" t="s">
         <v>658</v>
-      </c>
-      <c r="B320" s="15" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" s="16" t="s">
+        <v>659</v>
+      </c>
+      <c r="B321" s="15" t="s">
         <v>660</v>
-      </c>
-      <c r="B321" s="15" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" s="16" t="s">
+        <v>661</v>
+      </c>
+      <c r="B322" s="15" t="s">
         <v>662</v>
-      </c>
-      <c r="B322" s="15" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" s="16" t="s">
+        <v>663</v>
+      </c>
+      <c r="B323" s="15" t="s">
         <v>664</v>
-      </c>
-      <c r="B323" s="15" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="B324" s="15" t="s">
         <v>666</v>
-      </c>
-      <c r="B324" s="15" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" s="16" t="s">
+        <v>667</v>
+      </c>
+      <c r="B325" s="15" t="s">
         <v>668</v>
-      </c>
-      <c r="B325" s="15" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" s="16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B326" s="15" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" s="16" t="s">
+        <v>670</v>
+      </c>
+      <c r="B327" s="15" t="s">
         <v>671</v>
-      </c>
-      <c r="B327" s="15" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" s="16" t="s">
+        <v>672</v>
+      </c>
+      <c r="B328" s="15" t="s">
         <v>673</v>
-      </c>
-      <c r="B328" s="15" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" s="16" t="s">
+        <v>674</v>
+      </c>
+      <c r="B329" s="15" t="s">
         <v>675</v>
-      </c>
-      <c r="B329" s="15" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" s="16" t="s">
+        <v>676</v>
+      </c>
+      <c r="B330" s="15" t="s">
         <v>677</v>
-      </c>
-      <c r="B330" s="15" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" s="16" t="s">
+        <v>678</v>
+      </c>
+      <c r="B331" s="15" t="s">
         <v>679</v>
-      </c>
-      <c r="B331" s="15" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" s="16" t="s">
+        <v>680</v>
+      </c>
+      <c r="B332" s="15" t="s">
         <v>681</v>
-      </c>
-      <c r="B332" s="15" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" s="16" t="s">
+        <v>682</v>
+      </c>
+      <c r="B333" s="15" t="s">
         <v>683</v>
-      </c>
-      <c r="B333" s="15" t="s">
-        <v>684</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" s="16" t="s">
+        <v>684</v>
+      </c>
+      <c r="B334" s="15" t="s">
         <v>685</v>
-      </c>
-      <c r="B334" s="15" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" s="16" t="s">
+        <v>686</v>
+      </c>
+      <c r="B335" s="15" t="s">
         <v>687</v>
-      </c>
-      <c r="B335" s="15" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" s="16" t="s">
+        <v>688</v>
+      </c>
+      <c r="B336" s="15" t="s">
         <v>689</v>
-      </c>
-      <c r="B336" s="15" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" s="16" t="s">
+        <v>690</v>
+      </c>
+      <c r="B337" s="15" t="s">
         <v>691</v>
-      </c>
-      <c r="B337" s="15" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" s="16" t="s">
+        <v>692</v>
+      </c>
+      <c r="B338" s="15" t="s">
         <v>693</v>
-      </c>
-      <c r="B338" s="15" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" s="16" t="s">
+        <v>694</v>
+      </c>
+      <c r="B339" s="15" t="s">
         <v>695</v>
-      </c>
-      <c r="B339" s="15" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" s="16" t="s">
+        <v>696</v>
+      </c>
+      <c r="B340" s="15" t="s">
         <v>697</v>
-      </c>
-      <c r="B340" s="15" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" s="16" t="s">
+        <v>698</v>
+      </c>
+      <c r="B341" s="15" t="s">
         <v>699</v>
-      </c>
-      <c r="B341" s="15" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" s="16" t="s">
+        <v>700</v>
+      </c>
+      <c r="B342" s="15" t="s">
         <v>701</v>
-      </c>
-      <c r="B342" s="15" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" s="16" t="s">
+        <v>702</v>
+      </c>
+      <c r="B343" s="15" t="s">
         <v>703</v>
-      </c>
-      <c r="B343" s="15" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" s="16" t="s">
+        <v>704</v>
+      </c>
+      <c r="B344" s="15" t="s">
         <v>705</v>
-      </c>
-      <c r="B344" s="15" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" s="16" t="s">
+        <v>706</v>
+      </c>
+      <c r="B345" s="15" t="s">
         <v>707</v>
-      </c>
-      <c r="B345" s="15" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" s="16" t="s">
+        <v>708</v>
+      </c>
+      <c r="B346" s="15" t="s">
         <v>709</v>
-      </c>
-      <c r="B346" s="15" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" s="16" t="s">
+        <v>710</v>
+      </c>
+      <c r="B347" s="15" t="s">
         <v>711</v>
-      </c>
-      <c r="B347" s="15" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B348" s="15" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.2">
@@ -9381,15 +9381,87 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A287:A288"/>
-    <mergeCell ref="A289:A290"/>
-    <mergeCell ref="A308:A312"/>
-    <mergeCell ref="A277:A278"/>
-    <mergeCell ref="C277:C278"/>
-    <mergeCell ref="A279:A280"/>
-    <mergeCell ref="C279:C280"/>
-    <mergeCell ref="A284:A285"/>
-    <mergeCell ref="C284:C285"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="A129:A136"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A97:A100"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A148:A160"/>
+    <mergeCell ref="A161:A164"/>
+    <mergeCell ref="A165:A169"/>
+    <mergeCell ref="B165:B169"/>
+    <mergeCell ref="A171:A172"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="A184:A185"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="B186:B188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="A176:A177"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="A199:A201"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="A207:A208"/>
+    <mergeCell ref="C207:C208"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="A219:A220"/>
+    <mergeCell ref="C219:C220"/>
+    <mergeCell ref="A222:A223"/>
+    <mergeCell ref="B222:B223"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="C209:C210"/>
+    <mergeCell ref="A211:A212"/>
+    <mergeCell ref="A213:A214"/>
+    <mergeCell ref="C213:C214"/>
+    <mergeCell ref="A215:A216"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="C235:C236"/>
+    <mergeCell ref="A237:A238"/>
+    <mergeCell ref="C237:C238"/>
+    <mergeCell ref="A239:A241"/>
+    <mergeCell ref="A242:A249"/>
+    <mergeCell ref="A250:A253"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="A224:A226"/>
+    <mergeCell ref="B224:B226"/>
+    <mergeCell ref="A227:A229"/>
+    <mergeCell ref="B227:B229"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A235:A236"/>
     <mergeCell ref="A267:A268"/>
     <mergeCell ref="C267:C268"/>
     <mergeCell ref="A269:A270"/>
@@ -9404,87 +9476,15 @@
     <mergeCell ref="B261:B263"/>
     <mergeCell ref="A264:A266"/>
     <mergeCell ref="B264:B266"/>
-    <mergeCell ref="C235:C236"/>
-    <mergeCell ref="A237:A238"/>
-    <mergeCell ref="C237:C238"/>
-    <mergeCell ref="A239:A241"/>
-    <mergeCell ref="A242:A249"/>
-    <mergeCell ref="A250:A253"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="A224:A226"/>
-    <mergeCell ref="B224:B226"/>
-    <mergeCell ref="A227:A229"/>
-    <mergeCell ref="B227:B229"/>
-    <mergeCell ref="A230:A234"/>
-    <mergeCell ref="A235:A236"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="A219:A220"/>
-    <mergeCell ref="C219:C220"/>
-    <mergeCell ref="A222:A223"/>
-    <mergeCell ref="B222:B223"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="C209:C210"/>
-    <mergeCell ref="A211:A212"/>
-    <mergeCell ref="A213:A214"/>
-    <mergeCell ref="C213:C214"/>
-    <mergeCell ref="A215:A216"/>
-    <mergeCell ref="C215:C216"/>
-    <mergeCell ref="A199:A201"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="A202:A203"/>
-    <mergeCell ref="C202:C203"/>
-    <mergeCell ref="A207:A208"/>
-    <mergeCell ref="C207:C208"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="C191:C192"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="A186:A188"/>
-    <mergeCell ref="B186:B188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="C189:C190"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="A148:A160"/>
-    <mergeCell ref="A161:A164"/>
-    <mergeCell ref="A165:A169"/>
-    <mergeCell ref="B165:B169"/>
-    <mergeCell ref="A171:A172"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="A129:A136"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A97:A100"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="A287:A288"/>
+    <mergeCell ref="A289:A290"/>
+    <mergeCell ref="A308:A312"/>
+    <mergeCell ref="A277:A278"/>
+    <mergeCell ref="C277:C278"/>
+    <mergeCell ref="A279:A280"/>
+    <mergeCell ref="C279:C280"/>
+    <mergeCell ref="A284:A285"/>
+    <mergeCell ref="C284:C285"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>